<commit_message>
Preparing DB for the app.
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="197">
   <si>
     <t>QUERY</t>
   </si>
@@ -483,9 +483,6 @@
     <t>Xavi (Spain)</t>
   </si>
   <si>
-    <t>Which team was awarder with the 'FIFA Fair Play Trophy' in 2010?</t>
-  </si>
-  <si>
     <t>Which goalkeeper received the 'Golden Gloove' trophy for the best goalkeeper of the tournament in 2010?</t>
   </si>
   <si>
@@ -595,6 +592,21 @@
   </si>
   <si>
     <t>What was the name of the official match ball used during FIFA World Cup in Germany, 1974?</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>difficult</t>
+  </si>
+  <si>
+    <t>extreme</t>
+  </si>
+  <si>
+    <t>Which team was awarded with the 'FIFA Fair Play Trophy' in 2010?</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -952,23 +964,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="129.42578125" customWidth="1"/>
+    <col min="1" max="1" width="115.140625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,16 +998,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1010,11 +1023,20 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>196</v>
+      </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1030,11 +1052,20 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
+      <c r="F3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
+      </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1051,13 +1082,19 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1079,8 +1116,14 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1097,10 +1140,19 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1122,8 +1174,14 @@
       <c r="G7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1139,11 +1197,20 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
+      <c r="F8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G8" t="s">
+        <v>196</v>
+      </c>
       <c r="H8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1159,11 +1226,20 @@
       <c r="E9" t="s">
         <v>39</v>
       </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H9" t="s">
+        <v>196</v>
+      </c>
+      <c r="I9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1179,11 +1255,20 @@
       <c r="E10" t="s">
         <v>38</v>
       </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H10" t="s">
+        <v>196</v>
+      </c>
+      <c r="I10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1205,8 +1290,14 @@
       <c r="G11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1222,11 +1313,20 @@
       <c r="E12" t="s">
         <v>44</v>
       </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
       <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1248,8 +1348,14 @@
       <c r="G13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1266,10 +1372,19 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>196</v>
+      </c>
+      <c r="I14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1286,10 +1401,19 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>196</v>
+      </c>
+      <c r="I15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1306,10 +1430,19 @@
         <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>196</v>
+      </c>
+      <c r="I16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1325,11 +1458,20 @@
       <c r="E17" t="s">
         <v>59</v>
       </c>
+      <c r="F17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" t="s">
+        <v>196</v>
+      </c>
       <c r="H17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1346,10 +1488,19 @@
         <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>196</v>
+      </c>
+      <c r="I18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1366,10 +1517,19 @@
         <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>196</v>
+      </c>
+      <c r="I19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1386,10 +1546,19 @@
         <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>196</v>
+      </c>
+      <c r="I20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1406,10 +1575,19 @@
         <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>196</v>
+      </c>
+      <c r="I21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1431,8 +1609,14 @@
       <c r="G22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>196</v>
+      </c>
+      <c r="I22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -1448,11 +1632,20 @@
       <c r="E23" t="s">
         <v>80</v>
       </c>
+      <c r="F23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G23" t="s">
+        <v>196</v>
+      </c>
       <c r="H23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1468,11 +1661,20 @@
       <c r="E24" t="s">
         <v>64</v>
       </c>
+      <c r="F24" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" t="s">
+        <v>196</v>
+      </c>
       <c r="H24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1488,11 +1690,20 @@
       <c r="E25" t="s">
         <v>87</v>
       </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
       <c r="G25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H25" t="s">
+        <v>196</v>
+      </c>
+      <c r="I25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -1508,11 +1719,20 @@
       <c r="E26" t="s">
         <v>79</v>
       </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
       <c r="G26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H26" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -1528,11 +1748,20 @@
       <c r="E27" t="s">
         <v>95</v>
       </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
       <c r="G27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H27" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -1548,11 +1777,20 @@
       <c r="E28" t="s">
         <v>122</v>
       </c>
+      <c r="F28" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" t="s">
+        <v>196</v>
+      </c>
       <c r="H28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1569,13 +1807,19 @@
         <v>128</v>
       </c>
       <c r="F29" t="s">
+        <v>196</v>
+      </c>
+      <c r="G29" t="s">
         <v>13</v>
       </c>
       <c r="H29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -1597,8 +1841,14 @@
       <c r="G30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>196</v>
+      </c>
+      <c r="I30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>129</v>
       </c>
@@ -1614,11 +1864,20 @@
       <c r="E31" t="s">
         <v>35</v>
       </c>
+      <c r="F31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" t="s">
+        <v>196</v>
+      </c>
       <c r="H31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -1634,11 +1893,20 @@
       <c r="E32" t="s">
         <v>100</v>
       </c>
+      <c r="F32" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" t="s">
+        <v>196</v>
+      </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -1654,11 +1922,20 @@
       <c r="E33" t="s">
         <v>105</v>
       </c>
+      <c r="F33" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" t="s">
+        <v>196</v>
+      </c>
       <c r="H33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -1674,11 +1951,20 @@
       <c r="E34" t="s">
         <v>108</v>
       </c>
+      <c r="F34" t="s">
+        <v>196</v>
+      </c>
+      <c r="G34" t="s">
+        <v>196</v>
+      </c>
       <c r="H34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1694,11 +1980,20 @@
       <c r="E35" t="s">
         <v>118</v>
       </c>
+      <c r="F35" t="s">
+        <v>196</v>
+      </c>
+      <c r="G35" t="s">
+        <v>196</v>
+      </c>
       <c r="H35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1714,11 +2009,20 @@
       <c r="E36" t="s">
         <v>117</v>
       </c>
+      <c r="F36" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" t="s">
+        <v>196</v>
+      </c>
       <c r="H36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>134</v>
       </c>
@@ -1734,11 +2038,20 @@
       <c r="E37" t="s">
         <v>138</v>
       </c>
+      <c r="F37" t="s">
+        <v>196</v>
+      </c>
+      <c r="G37" t="s">
+        <v>196</v>
+      </c>
       <c r="H37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -1755,10 +2068,19 @@
         <v>79</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>141</v>
       </c>
@@ -1774,11 +2096,20 @@
       <c r="E39" t="s">
         <v>68</v>
       </c>
+      <c r="F39" t="s">
+        <v>196</v>
+      </c>
+      <c r="G39" t="s">
+        <v>196</v>
+      </c>
       <c r="H39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -1794,11 +2125,20 @@
       <c r="E40" t="s">
         <v>151</v>
       </c>
+      <c r="F40" t="s">
+        <v>196</v>
+      </c>
+      <c r="G40" t="s">
+        <v>196</v>
+      </c>
       <c r="H40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -1814,11 +2154,20 @@
       <c r="E41" t="s">
         <v>149</v>
       </c>
+      <c r="F41" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" t="s">
+        <v>196</v>
+      </c>
       <c r="H41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -1835,13 +2184,19 @@
         <v>148</v>
       </c>
       <c r="F42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" t="s">
         <v>13</v>
       </c>
       <c r="H42" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -1858,44 +2213,56 @@
         <v>151</v>
       </c>
       <c r="F43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" t="s">
         <v>13</v>
       </c>
       <c r="H43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
         <v>153</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F44" t="s">
+        <v>196</v>
+      </c>
+      <c r="G44" t="s">
         <v>13</v>
       </c>
       <c r="H44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D45" t="s">
         <v>64</v>
@@ -1904,15 +2271,21 @@
         <v>87</v>
       </c>
       <c r="F45" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" t="s">
         <v>13</v>
       </c>
       <c r="H45" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
         <v>65</v>
@@ -1926,173 +2299,254 @@
       <c r="E46" t="s">
         <v>36</v>
       </c>
+      <c r="F46" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" t="s">
+        <v>196</v>
+      </c>
       <c r="H46" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" t="s">
         <v>161</v>
       </c>
-      <c r="B47" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>162</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>163</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
+        <v>196</v>
+      </c>
+      <c r="G47" t="s">
+        <v>196</v>
+      </c>
+      <c r="H47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>164</v>
       </c>
-      <c r="H47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>165</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>166</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>167</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>168</v>
       </c>
-      <c r="E48" t="s">
-        <v>169</v>
+      <c r="F48" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48" t="s">
+        <v>196</v>
       </c>
       <c r="H48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E49" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" t="s">
+        <v>196</v>
+      </c>
+      <c r="G49" t="s">
+        <v>196</v>
+      </c>
+      <c r="H49" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>175</v>
-      </c>
-      <c r="H49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>176</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="F50" t="s">
+        <v>196</v>
+      </c>
+      <c r="G50" t="s">
+        <v>196</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
+        <v>178</v>
+      </c>
+      <c r="E51" t="s">
         <v>179</v>
       </c>
-      <c r="E51" t="s">
-        <v>180</v>
+      <c r="F51" t="s">
+        <v>196</v>
+      </c>
+      <c r="G51" t="s">
+        <v>196</v>
       </c>
       <c r="H51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E52" t="s">
+        <v>179</v>
+      </c>
+      <c r="F52" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" t="s">
+        <v>196</v>
+      </c>
+      <c r="H52" t="s">
+        <v>196</v>
+      </c>
+      <c r="I52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" t="s">
+        <v>196</v>
+      </c>
+      <c r="I53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" t="s">
         <v>180</v>
       </c>
-      <c r="G52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>191</v>
-      </c>
-      <c r="B53" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D54" t="s">
         <v>174</v>
       </c>
-      <c r="D53" t="s">
-        <v>183</v>
-      </c>
-      <c r="E53" t="s">
-        <v>175</v>
-      </c>
-      <c r="G53" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>184</v>
-      </c>
-      <c r="B54" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>181</v>
       </c>
-      <c r="D54" t="s">
-        <v>175</v>
-      </c>
-      <c r="E54" t="s">
-        <v>182</v>
+      <c r="F54" t="s">
+        <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H54" t="s">
+        <v>196</v>
+      </c>
+      <c r="I54" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55">
         <v>1970</v>
@@ -2106,28 +2560,46 @@
       <c r="E55">
         <v>1978</v>
       </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
       <c r="G55" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="H55" t="s">
+        <v>196</v>
+      </c>
+      <c r="I55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" t="s">
         <v>185</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>186</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>187</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>188</v>
       </c>
-      <c r="E56" t="s">
-        <v>189</v>
+      <c r="F56" t="s">
+        <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>13</v>
+        <v>196</v>
+      </c>
+      <c r="H56" t="s">
+        <v>196</v>
+      </c>
+      <c r="I56" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing DB for the app - continuation.
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -966,19 +966,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I68"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="115.140625" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>